<commit_message>
adjusted Zeitplan: added row 17(REST API...)
</commit_message>
<xml_diff>
--- a/Zeitplanxlsx.xlsx
+++ b/Zeitplanxlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\HF\Webtech2\Hotel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsobildung-my.sharepoint.com/personal/neven_kljajic_student_ipso_ch/Documents/6. Semester/Web-Technologie-2/Praxisprojekt_Webtechnologie_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508CA1F8-4D75-41BD-B122-4A4BE890A311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{508CA1F8-4D75-41BD-B122-4A4BE890A311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81AC370A-7E4D-429B-9A0D-DDC384B8D58C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{073B4FD5-DAC6-4240-91AB-836494C8A345}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{073B4FD5-DAC6-4240-91AB-836494C8A345}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Phase 1</t>
   </si>
@@ -180,6 +180,30 @@
   </si>
   <si>
     <t>NK</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.5</t>
+  </si>
+  <si>
+    <t>2.6</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>2.8</t>
+  </si>
+  <si>
+    <t>2.9</t>
+  </si>
+  <si>
+    <t>2.12</t>
+  </si>
+  <si>
+    <t>REST API für jedes Table</t>
   </si>
 </sst>
 </file>
@@ -548,26 +572,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50BA8BC4-CD1A-400B-9CD7-D0BFC9CC4662}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+      <selection activeCell="A17" sqref="A17:E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="53.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="53.26953125" customWidth="1"/>
+    <col min="3" max="3" width="25.453125" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -584,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1.1000000000000001</v>
       </c>
@@ -601,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -618,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1.3</v>
       </c>
@@ -635,7 +659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -652,7 +676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.5</v>
       </c>
@@ -669,7 +693,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.6</v>
       </c>
@@ -686,7 +710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1.7</v>
       </c>
@@ -703,7 +727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -720,18 +744,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="C11" s="1">
         <f>SUM(C3:C10)</f>
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -748,7 +772,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>2.1</v>
       </c>
@@ -762,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -779,7 +803,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -796,12 +820,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>2.4</v>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C17">
         <v>12</v>
@@ -810,261 +834,278 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="E17" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>2.4</v>
+      </c>
+      <c r="E18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>2.5</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
         <v>27</v>
       </c>
-      <c r="C18">
-        <v>12</v>
-      </c>
-      <c r="D18">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
       <c r="C19">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D19">
         <v>2.4</v>
       </c>
       <c r="E19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20">
+        <v>8</v>
+      </c>
+      <c r="D20">
+        <v>2.5</v>
+      </c>
+      <c r="E20" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>2.7</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
         <v>29</v>
       </c>
-      <c r="C20">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21">
+        <v>2.4</v>
+      </c>
+      <c r="E21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
         <v>30</v>
       </c>
-      <c r="C21">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>2.9</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
       <c r="C22">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D22" t="s">
         <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23">
         <v>12</v>
       </c>
-      <c r="D23">
-        <v>2.7</v>
+      <c r="D23" t="s">
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24">
         <v>12</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24">
+        <v>2.7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
         <v>31</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E25" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="C25" s="1">
-        <f>SUM(C14:C24)</f>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="C26" s="1">
+        <f>SUM(C14:C25)</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>2</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>3</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D28" t="s">
         <v>4</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E28" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>37</v>
       </c>
-      <c r="C28">
+      <c r="C29">
         <v>30</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>38</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" t="s">
-        <v>40</v>
       </c>
       <c r="C30">
         <v>3</v>
       </c>
       <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+      <c r="D31">
         <v>3.2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B31" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31">
-        <v>10</v>
-      </c>
-      <c r="D31">
-        <v>3.3</v>
       </c>
       <c r="E31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C32">
         <v>10</v>
       </c>
       <c r="D32">
-        <v>3.4</v>
+        <v>3.3</v>
       </c>
       <c r="E32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="C33" s="1">
-        <f>SUM(C28:C32)</f>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>3.4</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="2"/>
+      <c r="C34" s="1">
+        <f>SUM(C29:C33)</f>
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
-      <c r="C35">
-        <f>SUM(C11,C25,C33)</f>
-        <v>199</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>SUM(C11,C26,C34)</f>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>